<commit_message>
amending plots for pub version
</commit_message>
<xml_diff>
--- a/nf1g/surv/nf1-renaming dataset.xlsx
+++ b/nf1g/surv/nf1-renaming dataset.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uofutah.sharepoint.com/sites/HolmenLab/Shared Documents/General/garrett hl-onedrive/R/nf1/cohorts3/ds/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uofutah.sharepoint.com/sites/HolmenLab/Shared Documents/General/garrett hl-onedrive/R/rchpc/nf1g/surv/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="9" documentId="8_{2443A706-D482-4712-90D8-3B74E2D3726D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{54FDB4B1-B104-4600-B0FE-523BA6DD16B9}"/>
+  <xr:revisionPtr revIDLastSave="33" documentId="8_{2443A706-D482-4712-90D8-3B74E2D3726D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C61D0FBB-0E58-45F2-9CC8-9080C12555D6}"/>
   <bookViews>
-    <workbookView xWindow="14460" yWindow="2670" windowWidth="13335" windowHeight="14370" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="31590" yWindow="435" windowWidth="16380" windowHeight="14370" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="resultant_geno" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="72">
   <si>
     <t>resultant_geno</t>
   </si>
@@ -205,9 +205,6 @@
     <t>patho_cat2_name</t>
   </si>
   <si>
-    <t>ned</t>
-  </si>
-  <si>
     <t>hist_cat</t>
   </si>
   <si>
@@ -216,12 +213,39 @@
   <si>
     <t>No histological classification</t>
   </si>
+  <si>
+    <t>XH-NE</t>
+  </si>
+  <si>
+    <t>XH-E</t>
+  </si>
+  <si>
+    <t>Excluded from histology (event)</t>
+  </si>
+  <si>
+    <t>Excluded from histology (no event)</t>
+  </si>
+  <si>
+    <t>3.1</t>
+  </si>
+  <si>
+    <t>Pretumorigenic</t>
+  </si>
+  <si>
+    <t>3.1.5</t>
+  </si>
+  <si>
+    <t>Astrocytoma, diffuse, low-grade (Grade 1)</t>
+  </si>
+  <si>
+    <t>Glioma, grade 1</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -238,6 +262,13 @@
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="&quot;PT Serif&quot;"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -260,7 +291,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -268,6 +299,11 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -20529,10 +20565,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
@@ -20573,50 +20609,66 @@
       </c>
     </row>
     <row r="5" spans="1:2">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B7" s="3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
-      <c r="A6" s="1" t="s">
+    <row r="8" spans="1:2">
+      <c r="A8" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B8" s="3" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
-      <c r="A7" s="1" t="s">
+    <row r="9" spans="1:2">
+      <c r="A9" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B9" s="3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
-      <c r="A8" s="1" t="s">
+    <row r="10" spans="1:2">
+      <c r="A10" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B10" s="3" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
-      <c r="A9" s="1" t="s">
+    <row r="11" spans="1:2">
+      <c r="A11" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B11" s="3" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
-      <c r="A10" s="1" t="s">
+    <row r="12" spans="1:2">
+      <c r="A12" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B12" s="1" t="s">
         <v>27</v>
       </c>
     </row>
@@ -20630,9 +20682,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:B15"/>
+  <dimension ref="A1:B17"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
@@ -20688,74 +20742,90 @@
       </c>
     </row>
     <row r="7" spans="1:2">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B9" s="3" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
-      <c r="A8" s="4" t="s">
+    <row r="10" spans="1:2">
+      <c r="A10" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B10" s="3" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
-      <c r="A9" s="4" t="s">
+    <row r="11" spans="1:2">
+      <c r="A11" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B11" s="3" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
-      <c r="A10" s="4" t="s">
+    <row r="12" spans="1:2">
+      <c r="A12" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B12" s="3" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
-      <c r="A11" s="4" t="s">
+    <row r="13" spans="1:2">
+      <c r="A13" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B13" s="3" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
-      <c r="A12" s="4" t="s">
+    <row r="14" spans="1:2">
+      <c r="A14" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B14" s="3" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
-      <c r="A13" s="4" t="s">
+    <row r="15" spans="1:2">
+      <c r="A15" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B15" s="3" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="1:2">
-      <c r="A14" s="4" t="s">
+    <row r="16" spans="1:2">
+      <c r="A16" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="B16" s="3" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="15" spans="1:2">
-      <c r="A15" s="4" t="s">
+    <row r="17" spans="1:2">
+      <c r="A17" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="B17" s="3" t="s">
         <v>27</v>
       </c>
     </row>
@@ -20769,10 +20839,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
@@ -20782,7 +20852,7 @@
   <sheetData>
     <row r="1" spans="1:2" ht="12.75">
       <c r="A1" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>49</v>
@@ -20822,10 +20892,10 @@
     </row>
     <row r="6" spans="1:2" ht="12.75">
       <c r="A6" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="12.75">
@@ -20837,11 +20907,19 @@
       </c>
     </row>
     <row r="8" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A8" s="1" t="s">
-        <v>60</v>
+      <c r="A8" s="5" t="s">
+        <v>64</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>27</v>
+      <c r="B8" s="5" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A9" t="s">
+        <v>63</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>66</v>
       </c>
     </row>
   </sheetData>

</xml_diff>